<commit_message>
try to implement sigmoid function (in second worksheet)
</commit_message>
<xml_diff>
--- a/data/Test function.xlsx
+++ b/data/Test function.xlsx
@@ -4,48 +4,75 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="23955" windowHeight="16680"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="23955" windowHeight="16680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sigmoid" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$D$4:$D$6</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Sigmoid!$E$13:$E$16</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$E$33</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Sigmoid!$F$108</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Time</t>
   </si>
@@ -75,6 +102,36 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>c/(1.0+Math.exp(a*x+b)))+d</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>pred</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>Sum:</t>
   </si>
 </sst>
 </file>
@@ -132,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,11 +601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255164416"/>
-        <c:axId val="255165952"/>
+        <c:axId val="182754304"/>
+        <c:axId val="183767808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="255164416"/>
+        <c:axId val="182754304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,12 +615,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255165952"/>
+        <c:crossAx val="183767808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255165952"/>
+        <c:axId val="183767808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +631,309 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255164416"/>
+        <c:crossAx val="182754304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sigmoid!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>freq</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sigmoid!$C$20:$C$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="88"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.00000000000028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>281.00000000000398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>393.99999999999602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>458.99999999999983</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>503.00000000000028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576.99999999999591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>605.99999999999886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>664.99999999999682</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>761.9999999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>882.00000000000364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1007.9999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sigmoid!$D$20:$D$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="88"/>
+                <c:pt idx="0">
+                  <c:v>59.349820927056697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.345579861379498</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.340549844116303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.329626136919899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.298678209785798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.256739584138501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.201874726237399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.144242096312901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.107409239648497</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.080398855994403</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.074968436783301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.073463193424502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sigmoid!$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pred</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sigmoid!$C$20:$C$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="88"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.00000000000028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>281.00000000000398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>393.99999999999602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>458.99999999999983</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>503.00000000000028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576.99999999999591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>605.99999999999886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>664.99999999999682</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>761.9999999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>882.00000000000364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1007.9999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sigmoid!$E$20:$E$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="88"/>
+                <c:pt idx="0">
+                  <c:v>59.216945367205412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.216945367203834</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.216945367202356</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.216945367201127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.216945367200417</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.216945367199941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.216945367199131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.216945367198818</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.216945367198171</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.21694536719712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.216945367195812</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.216945367194441</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="270428032"/>
+        <c:axId val="270426496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="270428032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="270426496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="270426496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="270428032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -609,6 +969,41 @@
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -919,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -1486,13 +1881,283 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C7:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2.6416997531916215E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>19.999999520807446</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>20.000000023350488</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>59.216945325982323</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <f>SUM(F20:F31)</f>
+        <v>0.14734219306987334</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>59.349820927056697</v>
+      </c>
+      <c r="E20">
+        <f>($E$15/(1+EXP($E$13*C20+$E$14)))+$E$16</f>
+        <v>59.216945367205412</v>
+      </c>
+      <c r="F20">
+        <f>POWER(E20-D20,2)</f>
+        <v>1.7655914405792589E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>145.00000000000028</v>
+      </c>
+      <c r="D21">
+        <v>59.345579861379498</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E84" si="0">($E$15/(1+EXP($E$13*C21+$E$14)))+$E$16</f>
+        <v>59.216945367203834</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F84" si="1">POWER(E21-D21,2)</f>
+        <v>1.6546833091828899E-2</v>
+      </c>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>281.00000000000398</v>
+      </c>
+      <c r="D22">
+        <v>59.340549844116303</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>59.216945367202356</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1.5278066713170413E-2</v>
+      </c>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>393.99999999999602</v>
+      </c>
+      <c r="D23">
+        <v>59.329626136919899</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>59.216945367201127</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1.2696955864414812E-2</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>458.99999999999983</v>
+      </c>
+      <c r="D24">
+        <v>59.298678209785798</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>59.216945367200417</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>6.6802575570867684E-3</v>
+      </c>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>503.00000000000028</v>
+      </c>
+      <c r="D25">
+        <v>59.256739584138501</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>59.216945367199941</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1.5835797017531845E-3</v>
+      </c>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>576.99999999999591</v>
+      </c>
+      <c r="D26">
+        <v>59.201874726237399</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>59.216945367199131</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>2.2712421899741589E-4</v>
+      </c>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>605.99999999999886</v>
+      </c>
+      <c r="D27">
+        <v>59.144242096312901</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>59.216945367198818</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>5.2857655975110255E-3</v>
+      </c>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>664.99999999999682</v>
+      </c>
+      <c r="D28">
+        <v>59.107409239648497</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>59.216945367198171</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1.1998163238578503E-2</v>
+      </c>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>761.9999999999992</v>
+      </c>
+      <c r="D29">
+        <v>59.080398855994403</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>59.21694536719712</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>1.8644949721633625E-2</v>
+      </c>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>882.00000000000364</v>
+      </c>
+      <c r="D30">
+        <v>59.074968436783301</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>59.216945367195812</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>2.0157448769359029E-2</v>
+      </c>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1007.9999999999994</v>
+      </c>
+      <c r="D31">
+        <v>59.073463193424502</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>59.216945367194441</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>2.0587134189747096E-2</v>
+      </c>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
include coefficients calculated in DopplerCurve.java
</commit_message>
<xml_diff>
--- a/data/Test function.xlsx
+++ b/data/Test function.xlsx
@@ -607,11 +607,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179370240"/>
-        <c:axId val="178978816"/>
+        <c:axId val="312687616"/>
+        <c:axId val="312689408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179370240"/>
+        <c:axId val="312687616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,12 +621,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178978816"/>
+        <c:crossAx val="312689408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178978816"/>
+        <c:axId val="312689408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179370240"/>
+        <c:crossAx val="312687616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -842,34 +842,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>150.9906365731448</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150.89285525391014</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150.69697702764554</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150.50068482356573</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.30398687405466</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149.94893464492682</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149.73134536303553</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>149.57281452179473</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>149.37432200421728</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>149.29482442363363</c:v>
+                  <c:v>150.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,11 +884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179041024"/>
-        <c:axId val="179042560"/>
+        <c:axId val="313624064"/>
+        <c:axId val="313625600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179041024"/>
+        <c:axId val="313624064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,12 +898,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179042560"/>
+        <c:crossAx val="313625600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179042560"/>
+        <c:axId val="313625600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179041024"/>
+        <c:crossAx val="313624064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1865,7 +1865,7 @@
   <dimension ref="C7:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,7 +1880,7 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>4.923431479352364E-3</v>
+        <v>-318.18</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="13">
-        <v>-0.45034145353262867</v>
+        <v>-95.68</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
@@ -1896,7 +1896,7 @@
         <v>13</v>
       </c>
       <c r="E15">
-        <v>83.492602115418819</v>
+        <v>60.44</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>14</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>89.6</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H17">
         <f>SUM(F20:F31)</f>
-        <v>0.19078309775599453</v>
+        <v>3.8543960000000008</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
@@ -1939,11 +1939,11 @@
       </c>
       <c r="E20">
         <f>($E$15/(1+EXP($E$13*C20+$E$14)))+$E$16</f>
-        <v>150.9906365731448</v>
+        <v>150.04</v>
       </c>
       <c r="F20">
         <f>POWER(E20-D20,2)</f>
-        <v>4.106158077586252E-2</v>
+        <v>0.5595040000000282</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
@@ -1954,12 +1954,12 @@
         <v>150.77699999999999</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E31" si="0">($E$15/(1+EXP($E$13*C21+$E$14)))+$E$16</f>
-        <v>150.89285525391014</v>
+        <f t="shared" ref="E21:E29" si="0">($E$15/(1+EXP($E$13*C21+$E$14)))+$E$16</f>
+        <v>150.04</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F31" si="1">POWER(E21-D21,2)</f>
-        <v>1.3422439858586472E-2</v>
+        <f t="shared" ref="F21:F29" si="1">POWER(E21-D21,2)</f>
+        <v>0.54316899999999224</v>
       </c>
       <c r="I21" s="12"/>
     </row>
@@ -1972,11 +1972,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>150.69697702764554</v>
+        <v>150.04</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>2.2111599290478251E-3</v>
+        <v>0.49561600000001088</v>
       </c>
       <c r="I22" s="12"/>
     </row>
@@ -1989,11 +1989,11 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>150.50068482356573</v>
+        <v>150.04</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>3.3238823558254742E-2</v>
+        <v>0.4134490000000009</v>
       </c>
       <c r="I23" s="12"/>
     </row>
@@ -2006,11 +2006,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>150.30398687405466</v>
+        <v>150.04</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>6.7606825663864584E-2</v>
+        <v>0.27457600000000093</v>
       </c>
       <c r="I24" s="12"/>
     </row>
@@ -2023,13 +2023,16 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>149.94893464492682</v>
+        <v>150.04</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>7.9326374743131194E-3</v>
-      </c>
-      <c r="I25" s="12"/>
+        <v>3.9999999999245122E-6</v>
+      </c>
+      <c r="I25" s="13">
+        <f>AVERAGE(D20:D29)</f>
+        <v>150.13079999999999</v>
+      </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26">
@@ -2040,11 +2043,11 @@
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>149.73134536303553</v>
+        <v>150.04</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>8.7133568002338724E-3</v>
+        <v>0.1616039999999894</v>
       </c>
       <c r="I26" s="12"/>
     </row>
@@ -2057,11 +2060,11 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>149.57281452179473</v>
+        <v>150.04</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>1.4355519632898116E-2</v>
+        <v>0.34456899999998719</v>
       </c>
       <c r="I27" s="12"/>
     </row>
@@ -2074,11 +2077,11 @@
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>149.37432200421728</v>
+        <v>150.04</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>2.2393720831401136E-3</v>
+        <v>0.5083689999999913</v>
       </c>
       <c r="I28" s="12"/>
     </row>
@@ -2091,11 +2094,11 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>149.29482442363363</v>
+        <v>150.04</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>1.3819797931543831E-6</v>
+        <v>0.55353599999999969</v>
       </c>
       <c r="I29" s="12"/>
     </row>

</xml_diff>

<commit_message>
include sample that got optimised in Java
</commit_message>
<xml_diff>
--- a/data/Test function.xlsx
+++ b/data/Test function.xlsx
@@ -4,72 +4,106 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="23955" windowHeight="16680" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="23955" windowHeight="16680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sigmoid" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$D$4:$D$6</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet2!$C$1:$C$4</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sigmoid!$E$13:$E$16</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0000001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Sheet2!$C$1:$C$4</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sigmoid!$E$13:$E$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Sheet2!$C$1:$C$4</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sigmoid!$E$13:$E$16</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$E$33</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet2!$C$6</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sigmoid!$H$17</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">80</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">-80</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">-100</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -77,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -137,6 +171,15 @@
   </si>
   <si>
     <t>Sum:</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Pred</t>
   </si>
 </sst>
 </file>
@@ -607,11 +650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="312687616"/>
-        <c:axId val="312689408"/>
+        <c:axId val="308034560"/>
+        <c:axId val="308036352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="312687616"/>
+        <c:axId val="308034560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,12 +664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="312689408"/>
+        <c:crossAx val="308036352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="312689408"/>
+        <c:axId val="308036352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,13 +680,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="312687616"/>
+        <c:crossAx val="308034560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -842,7 +886,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>150.04</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>150.04</c:v>
@@ -884,11 +928,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313624064"/>
-        <c:axId val="313625600"/>
+        <c:axId val="308971008"/>
+        <c:axId val="308972544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313624064"/>
+        <c:axId val="308971008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,12 +942,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="313625600"/>
+        <c:crossAx val="308972544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="313625600"/>
+        <c:axId val="308972544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +958,309 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="313624064"/>
+        <c:crossAx val="308971008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Freq</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$9:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.82</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$9:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>59.349820927056697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.345579861379498</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.340549844116303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.329626136919899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.298678209785798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.256739584138501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.201874726237399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.144242096312901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.107409239648497</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.080398855994403</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.074968436783301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.073463193424502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pred</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$9:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.82</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$9:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>59.345968308140371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.345663556451662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.342943298870843</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.327809951780793</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.299436103686403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.265215417247241</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.187279482945932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.158109821352788</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.114646189687726</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.084971298003921</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.077306005399905</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.076168200056031</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="291042816"/>
+        <c:axId val="291041280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="291042816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="291041280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="291041280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="291042816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -985,6 +1331,41 @@
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1864,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,7 +2294,7 @@
       </c>
       <c r="H17">
         <f>SUM(F20:F31)</f>
-        <v>3.8543960000000008</v>
+        <v>22740.315836000005</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
@@ -1937,13 +2318,13 @@
       <c r="D20">
         <v>150.78800000000001</v>
       </c>
-      <c r="E20">
-        <f>($E$15/(1+EXP($E$13*C20+$E$14)))+$E$16</f>
-        <v>150.04</v>
+      <c r="E20" t="b">
+        <f>Sheet2!C9=($E$15/(1+EXP($E$13*C20+$E$14)))+$E$16</f>
+        <v>0</v>
       </c>
       <c r="F20">
         <f>POWER(E20-D20,2)</f>
-        <v>0.5595040000000282</v>
+        <v>22737.020944000004</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
@@ -2110,6 +2491,281 @@
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I32" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1">
+        <v>-1.63</v>
+      </c>
+      <c r="F1">
+        <v>-1.63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="F2" s="13">
+        <v>9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>-0.27</v>
+      </c>
+      <c r="F3">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>59.345999999999997</v>
+      </c>
+      <c r="F4">
+        <v>59.345999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <f>SUM(D9:D57)</f>
+        <v>5.8768786578652953E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>59.349820927056697</v>
+      </c>
+      <c r="C9">
+        <f>($C$3/(1+EXP($C$1*A9+$C$2)))+$C$4</f>
+        <v>59.345968308140371</v>
+      </c>
+      <c r="D9">
+        <f>POWER(C9-B9,2)</f>
+        <v>1.4842672514435834E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.45</v>
+      </c>
+      <c r="B10">
+        <v>59.345579861379498</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C57" si="0">($C$3/(1+EXP($C$1*A10+$C$2)))+$C$4</f>
+        <v>59.345663556451662</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:D57" si="1">POWER(C10-B10,2)</f>
+        <v>7.0048651044428662E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2.81</v>
+      </c>
+      <c r="B11">
+        <v>59.340549844116303</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>59.342943298870843</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>5.7286256620274894E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.94</v>
+      </c>
+      <c r="B12">
+        <v>59.329626136919899</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>59.327809951780793</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>3.298528459508179E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.59</v>
+      </c>
+      <c r="B13">
+        <v>59.298678209785798</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>59.299436103686403</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>5.7440316457458141E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.03</v>
+      </c>
+      <c r="B14">
+        <v>59.256739584138501</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>59.265215417247241</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>7.1839746887213265E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5.77</v>
+      </c>
+      <c r="B15">
+        <v>59.201874726237399</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>59.187279482945932</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2.1302112673710915E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6.06</v>
+      </c>
+      <c r="B16">
+        <v>59.144242096312901</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>59.158109821352788</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1.9231379778191141E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6.65</v>
+      </c>
+      <c r="B17">
+        <v>59.107409239648497</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>59.114646189687726</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>5.2373445870288202E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7.62</v>
+      </c>
+      <c r="B18">
+        <v>59.080398855994403</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>59.084971298003921</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2.0907225930408118E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8.82</v>
+      </c>
+      <c r="B19">
+        <v>59.074968436783301</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>59.077306005399905</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>5.4642270373290933E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10.08</v>
+      </c>
+      <c r="B20">
+        <v>59.073463193424502</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>59.076168200056031</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>7.3170608766198017E-6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>